<commit_message>
Updated testcase and fixed test
</commit_message>
<xml_diff>
--- a/brmo-loader/src/test/resources/nl/b3p/brmo/loader/checks/overzicht_klein.xlsx
+++ b/brmo-loader/src/test/resources/nl/b3p/brmo/loader/checks/overzicht_klein.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t xml:space="preserve">AFGT_KLANTNUMMER</t>
   </si>
@@ -40,117 +40,137 @@
     <t xml:space="preserve">AFGT_IND_GELEVERD_VIA_URL</t>
   </si>
   <si>
-    <t xml:space="preserve">0000018301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9700004600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 09:36:35,007000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-YSK00G738-20190224-1.zip</t>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-06-2019 01:50:58,355000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-OOI00G451-20190615-1.zip</t>
   </si>
   <si>
     <t xml:space="preserve">J</t>
   </si>
   <si>
-    <t xml:space="preserve">21-03-2019 09:36:35,604000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-YSK00G5975-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:20:31,979000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-GOE00AB1340-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:29:03,681000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-GOE00U617-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:29:07,205000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-GOE00V1200-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:36:34,886000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-GOE00C5609A37-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:39:07,371000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-KPL01E3183A11-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:40:24,673000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-VSG00I2509A51-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:43:13,105000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-BNS00H454-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:43:53,882000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-BWH00N1015A12-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:44:29,994000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-MTD03N1852A84-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:46:30,781000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-VSG00I2510A20-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:49:21,565000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-OBG00EB2903-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:56:59,695000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-KGN00N730-20190224-1.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2019 11:57:18,291000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUTBX01-OBG00EH39-20190224-1.zip</t>
+    <t xml:space="preserve">9700005117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-06-2019 01:56:11,674000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-NMG00B6263-20190615-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-06-2019 01:56:12,150000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-NMG00C5206-20190615-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-06-2019 01:54:58,422000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-HVR00P2895-20190615-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-06-2019 01:47:50,511000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-PTE00C1380-20190615-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 04:10:08,199000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-VRE00G3100-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 04:10:08,948000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-VRE00G3112-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 04:09:59,527000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-SDT00K3787-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 04:10:08,282000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-VRE00G3111-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 04:10:08,823000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-VRE00G3110-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-10-2018 04:33:22,927000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-ANM00I604-20181010-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08-10-2018 20:19:31,533000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-ANM00I604-20180924-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-10-2018 10:16:56,788000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-ANM00I604-20181002-2.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-10-2018 10:14:51,981000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-ANM00I604-20181002-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-10-2018 04:42:16,174000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-ANM00I604-20181010-2.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 01:40:36,081000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-GLN00H1357-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 00:50:45,422000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-HEE01D2543-20190612-1.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-06-2019 01:39:53,612000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BKE-MUTBX01-GLN00H1358-20190612-1.zip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -173,6 +193,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,12 +242,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,15 +280,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F16"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.82"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,28 +319,28 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2" t="n">
+        <v>9700005117</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="2" t="n">
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -312,18 +349,18 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -332,18 +369,18 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+      <c r="A5" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -352,18 +389,18 @@
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
+      <c r="A6" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -372,18 +409,18 @@
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
+      <c r="A7" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
@@ -392,18 +429,18 @@
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
+      <c r="A8" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -412,18 +449,18 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
+      <c r="A9" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -432,18 +469,18 @@
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
+      <c r="A10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
@@ -452,18 +489,18 @@
         <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
+      <c r="A11" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>27</v>
@@ -472,18 +509,18 @@
         <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
+      <c r="A12" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>29</v>
@@ -492,18 +529,18 @@
         <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
+      <c r="A13" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>31</v>
@@ -512,18 +549,18 @@
         <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
+      <c r="A14" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>33</v>
@@ -532,18 +569,18 @@
         <v>34</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>7</v>
+      <c r="A15" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>35</v>
@@ -552,18 +589,18 @@
         <v>36</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
+      <c r="A16" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>37</v>
@@ -572,11 +609,75 @@
         <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>